<commit_message>
Corrected the schema provided by file.
</commit_message>
<xml_diff>
--- a/examples/demoday/data/example_product.xlsx
+++ b/examples/demoday/data/example_product.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="140">
   <si>
     <t xml:space="preserve">Dataset Metadata</t>
   </si>
@@ -341,12 +341,6 @@
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssn</t>
-  </si>
-  <si>
     <t xml:space="preserve">StreetNumber</t>
   </si>
   <si>
@@ -375,15 +369,6 @@
   </si>
   <si>
     <t xml:space="preserve">postalcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">PhoneNum</t>
@@ -850,7 +835,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1240,7 +1225,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,7 +1238,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1457,7 +1442,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>107</v>
@@ -1527,7 +1512,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>117</v>
@@ -1538,58 +1523,70 @@
         <v>118</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="F16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="23" t="n">
+        <v>20</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="F17" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C18" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="E18" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>124</v>
+      <c r="F18" s="22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="23" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>100</v>
@@ -1597,7 +1594,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>78</v>
@@ -1609,7 +1606,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F20" s="22" t="s">
         <v>100</v>
@@ -1617,50 +1614,50 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>78</v>
-      </c>
       <c r="C21" s="23" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E21" s="22" t="s">
         <v>130</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="C22" s="23" t="n">
         <v>100</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>133</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>134</v>
       </c>
       <c r="C23" s="23" t="n">
         <v>10</v>
@@ -1669,10 +1666,10 @@
         <v>98</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,61 +1677,23 @@
         <v>137</v>
       </c>
       <c r="B24" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="22" t="s">
+      <c r="F24" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="23" t="n">
-        <v>13</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>144</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>